<commit_message>
rebuilding site Sun Nov 22 15:08:07 CET 2020
</commit_message>
<xml_diff>
--- a/files/EXCEL_ALL_1_TO_15/G15.xlsx
+++ b/files/EXCEL_ALL_1_TO_15/G15.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chiara/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chiara/Desktop/Econometrie_MBF/G15/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{856D6159-6506-B041-B53A-987606351D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CEB8C6-3301-644E-85EB-C6163CE59666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15540" xr2:uid="{B7B1CEF5-BA87-644E-9F5E-805A86F966C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Baremme de correction</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>General Comments:</t>
+  </si>
+  <si>
+    <t>Good job! I think is clear and is intresting but might be too general to gather a proper effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The error of the task was in the choice of the frequency. When you choose days and you want to test the effect in the medium term (almost a year with 300 observations) is not compatible. Look the resource i made available in EPI on event study in finance, you will see why. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is not clear why you expect to see something that might have opposed effect. China and goldman sachs are going to go to the opposite side following your explanation. So it`s not completely clear. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think you did a great job here and is a pleasure to see that you are able to do this tasks using the material from the course. Its a good job! </t>
   </si>
 </sst>
 </file>
@@ -411,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -434,20 +446,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,26 +457,45 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,7 +814,7 @@
   <dimension ref="B2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,30 +828,30 @@
   <sheetData>
     <row r="2" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="19"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="22"/>
+      <c r="F4" s="18"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3" t="s">
         <v>46</v>
@@ -842,10 +861,10 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="22"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="5" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -853,7 +872,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="22"/>
+      <c r="F5" s="18"/>
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -861,23 +880,23 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="22"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="20">
         <v>44153</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="21">
         <f>E9/D8*20</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="22"/>
+        <v>16.833333333333336</v>
+      </c>
+      <c r="F6" s="18"/>
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -885,16 +904,16 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="22"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="22"/>
+      <c r="F7" s="18"/>
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -902,20 +921,20 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="22"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="22">
         <v>6</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="22"/>
+      <c r="F8" s="18"/>
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -923,7 +942,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="22"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
@@ -936,9 +955,9 @@
       </c>
       <c r="E9" s="3">
         <f>E11+E16+E20+E23</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="22"/>
+        <v>5.0500000000000007</v>
+      </c>
+      <c r="F9" s="18"/>
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -946,22 +965,22 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="22"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="18"/>
       <c r="H10" s="2"/>
       <c r="I10" s="3" t="s">
         <v>42</v>
@@ -971,7 +990,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="22"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
@@ -986,17 +1005,19 @@
       </c>
       <c r="E11" s="9">
         <f>SUM(E12:E15)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="22"/>
+        <v>1.85</v>
+      </c>
+      <c r="F11" s="18"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="22"/>
+      <c r="I11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="18"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
@@ -1008,16 +1029,18 @@
       <c r="D12" s="3">
         <v>0.5</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="18"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="22"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="18"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -1029,16 +1052,18 @@
       <c r="D13" s="3">
         <v>0.5</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="18"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="22"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="18"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
@@ -1050,16 +1075,18 @@
       <c r="D14" s="3">
         <v>0.5</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="22"/>
+      <c r="E14" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="18"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="22"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="18"/>
     </row>
     <row r="15" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -1071,16 +1098,18 @@
       <c r="D15" s="3">
         <v>0.5</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="22"/>
+      <c r="E15" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="F15" s="18"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="22"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="18"/>
     </row>
     <row r="16" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
@@ -1095,9 +1124,9 @@
       </c>
       <c r="E16" s="9">
         <f>SUM(E17:E19)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="22"/>
+        <v>1.3</v>
+      </c>
+      <c r="F16" s="18"/>
       <c r="H16" s="2"/>
       <c r="I16" s="3" t="s">
         <v>43</v>
@@ -1107,7 +1136,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="22"/>
+      <c r="O16" s="18"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
@@ -1119,16 +1148,20 @@
       <c r="D17" s="3">
         <v>0.5</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="22"/>
+      <c r="E17" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="F17" s="18"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="22"/>
+      <c r="I17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="18"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -1140,16 +1173,18 @@
       <c r="D18" s="3">
         <v>0.5</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="22"/>
+      <c r="E18" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="18"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="22"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="18"/>
     </row>
     <row r="19" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -1161,16 +1196,18 @@
       <c r="D19" s="5">
         <v>0.5</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="22"/>
+      <c r="E19" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="F19" s="18"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="22"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="18"/>
     </row>
     <row r="20" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
@@ -1185,9 +1222,9 @@
       </c>
       <c r="E20" s="9">
         <f>SUM(E21:E22)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="22"/>
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="18"/>
       <c r="H20" s="2"/>
       <c r="I20" s="3" t="s">
         <v>44</v>
@@ -1197,7 +1234,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="22"/>
+      <c r="O20" s="18"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -1209,16 +1246,20 @@
       <c r="D21" s="3">
         <v>0.5</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="22"/>
+      <c r="E21" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="18"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="22"/>
+      <c r="I21" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="18"/>
     </row>
     <row r="22" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -1230,16 +1271,18 @@
       <c r="D22" s="5">
         <v>0.5</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="22"/>
+      <c r="E22" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="18"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="22"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="18"/>
     </row>
     <row r="23" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
@@ -1254,9 +1297,9 @@
       </c>
       <c r="E23" s="9">
         <f>SUM(E24:E26)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="22"/>
+        <v>1.5</v>
+      </c>
+      <c r="F23" s="18"/>
       <c r="H23" s="2"/>
       <c r="I23" s="3" t="s">
         <v>45</v>
@@ -1266,7 +1309,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="22"/>
+      <c r="O23" s="18"/>
     </row>
     <row r="24" spans="2:15" ht="34" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
@@ -1278,16 +1321,20 @@
       <c r="D24" s="3">
         <v>0.5</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="22"/>
+      <c r="E24" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="18"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="22"/>
+      <c r="I24" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="18"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
@@ -1299,16 +1346,18 @@
       <c r="D25" s="3">
         <v>0.5</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="22"/>
+      <c r="E25" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="18"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="22"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="18"/>
     </row>
     <row r="26" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -1320,23 +1369,25 @@
       <c r="D26" s="5">
         <v>0.5</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="22"/>
+      <c r="E26" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="18"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="22"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="18"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="22"/>
+      <c r="F27" s="18"/>
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -1344,14 +1395,14 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="22"/>
+      <c r="O27" s="18"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="22"/>
+      <c r="F28" s="18"/>
       <c r="H28" s="2"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -1359,14 +1410,14 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="22"/>
+      <c r="O28" s="18"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="22"/>
+      <c r="F29" s="18"/>
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -1374,14 +1425,14 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="22"/>
+      <c r="O29" s="18"/>
     </row>
     <row r="30" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="23"/>
       <c r="H30" s="4"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -1389,16 +1440,16 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
-      <c r="O30" s="27"/>
+      <c r="O30" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I24:N26"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="I11:N15"/>
     <mergeCell ref="I17:N19"/>
     <mergeCell ref="I21:N22"/>
-    <mergeCell ref="I24:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>